<commit_message>
AV Arq de Comput ...... 06Jun2024
</commit_message>
<xml_diff>
--- a/03 Assessments/NOTAS AV - Arquitetura de Computador - 2024.1 Wyden UniRuy.xlsx
+++ b/03 Assessments/NOTAS AV - Arquitetura de Computador - 2024.1 Wyden UniRuy.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heleno\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YduqsArea1\22 WydenArea1ArquiteturaComputadores\03 Assessments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519E102B-2D93-4193-BF2B-E410464048AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6ED0D8-2109-451E-A962-89E8FC8879CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{413AB662-3705-4BE9-8AD4-FDF0F3F54212}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="86">
   <si>
     <t>201951145844 - ADERVAL SANTIAGO LEITE</t>
   </si>
@@ -288,6 +288,12 @@
   </si>
   <si>
     <t>Não criou conta no github</t>
+  </si>
+  <si>
+    <t>ATRASADO</t>
+  </si>
+  <si>
+    <t>GitHub - Durvalneto/Trabalho-Arquitetura-de-computadores-Prof.-Heleno; não entregou MAPA MENTAL</t>
   </si>
 </sst>
 </file>
@@ -585,10 +591,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="43" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
@@ -927,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2841AE5-15C3-4767-A901-0C645FE8FC21}">
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -942,13 +948,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
@@ -1257,14 +1263,17 @@
         <v>5</v>
       </c>
       <c r="E14" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F14" s="15">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>80</v>
+        <v>84</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1305,14 +1314,14 @@
         <v>1</v>
       </c>
       <c r="D16" s="18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E16" s="4">
         <v>3</v>
       </c>
       <c r="F16" s="15">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5.4</v>
       </c>
       <c r="G16" s="1">
         <v>2</v>
@@ -1430,7 +1439,7 @@
       <c r="D21" s="4">
         <v>9</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="18">
         <v>0</v>
       </c>
       <c r="F21" s="15">
@@ -1631,7 +1640,7 @@
       <c r="D29" s="4">
         <v>7</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="18">
         <v>0</v>
       </c>
       <c r="F29" s="15">
@@ -2027,7 +2036,7 @@
       <c r="E45" s="4">
         <v>4</v>
       </c>
-      <c r="F45" s="21" t="e">
+      <c r="F45" s="20" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
@@ -2367,6 +2376,7 @@
     <hyperlink ref="H57" r:id="rId12" display="https://github.com/Yan-Augusto2031/Trabalho" xr:uid="{CD76A79C-3766-429F-BD01-EA4FA711E6EA}"/>
     <hyperlink ref="H12" r:id="rId13" display="https://github.com/DLacerdadev/Arquitetura_Computadores" xr:uid="{56C2E7FD-32CB-4EA2-9470-D7BE7EFA66FD}"/>
     <hyperlink ref="H47" r:id="rId14" display="https://github.com/RafaCVarela/AvArquiteturadeComp" xr:uid="{A5710BDE-A1B0-4FA8-BCDB-3F32F0F54471}"/>
+    <hyperlink ref="H14" r:id="rId15" display="https://github.com/Durvalneto/Trabalho-Arquitetura-de-computadores-Prof.-Heleno" xr:uid="{910E6834-B017-455A-8B4E-EC79880BD007}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
NC Arq de Computador ... 11Jun2024
</commit_message>
<xml_diff>
--- a/03 Assessments/NOTAS AV - Arquitetura de Computador - 2024.1 Wyden UniRuy.xlsx
+++ b/03 Assessments/NOTAS AV - Arquitetura de Computador - 2024.1 Wyden UniRuy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YduqsArea1\22 WydenArea1ArquiteturaComputadores\03 Assessments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6ED0D8-2109-451E-A962-89E8FC8879CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9554E85A-6601-477E-A6F5-52FB91DA53D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{413AB662-3705-4BE9-8AD4-FDF0F3F54212}"/>
   </bookViews>
@@ -35,8 +35,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={B9A23567-296B-487D-8C14-9DC326CFF5AA}</author>
+  </authors>
+  <commentList>
+    <comment ref="D32" authorId="0" shapeId="0" xr:uid="{B9A23567-296B-487D-8C14-9DC326CFF5AA}">
+      <text>
+        <t>[Comentário encadeado]
+Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
+Comentário:
+    Fez NC e nem era para ter feito 10/06/2024</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="87">
   <si>
     <t>201951145844 - ADERVAL SANTIAGO LEITE</t>
   </si>
@@ -294,6 +312,9 @@
   </si>
   <si>
     <t>GitHub - Durvalneto/Trabalho-Arquitetura-de-computadores-Prof.-Heleno; não entregou MAPA MENTAL</t>
+  </si>
+  <si>
+    <t>NC = 6, prezevar a maior nota</t>
   </si>
 </sst>
 </file>
@@ -303,7 +324,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,6 +359,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -612,6 +639,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="HELENO CARDOSO DA SILVA FILHO" id="{DB3F4A37-8049-4460-8697-4AA805AAFE92}" userId="S::50891685553@professores.area1.edu.br::66a6a057-f068-4f0c-8462-27a0e682e1bd" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -929,12 +962,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D32" dT="2024-06-11T12:46:53.05" personId="{DB3F4A37-8049-4460-8697-4AA805AAFE92}" id="{B9A23567-296B-487D-8C14-9DC326CFF5AA}">
+    <text>Fez NC e nem era para ter feito 10/06/2024</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2841AE5-15C3-4767-A901-0C645FE8FC21}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2841AE5-15C3-4767-A901-0C645FE8FC21}">
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1650,6 +1691,9 @@
       <c r="G29" s="7" t="s">
         <v>80</v>
       </c>
+      <c r="H29" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
@@ -1710,14 +1754,14 @@
         <v>0.9</v>
       </c>
       <c r="D32" s="18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E32" s="4">
         <v>4</v>
       </c>
       <c r="F32" s="15">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5.8</v>
       </c>
       <c r="G32" s="1">
         <v>9</v>
@@ -2379,5 +2423,6 @@
     <hyperlink ref="H14" r:id="rId15" display="https://github.com/Durvalneto/Trabalho-Arquitetura-de-computadores-Prof.-Heleno" xr:uid="{910E6834-B017-455A-8B4E-EC79880BD007}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <legacyDrawing r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>